<commit_message>
matieral prep for meeting O2-CO2, hurricanes
</commit_message>
<xml_diff>
--- a/04_Output/rC_k600_edited.xlsx
+++ b/04_Output/rC_k600_edited.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\04_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CECF0-F0BE-45BB-B39F-6A29ECAF7F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEC8F28B-1F29-402B-8317-8493A916F424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="19">
   <si>
     <t>day</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>k600_1d</t>
+  </si>
+  <si>
+    <t>logQ</t>
   </si>
   <si>
     <t>13</t>
@@ -200,7 +203,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'13'!$I$1</c:f>
+              <c:f>'13'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -233,22 +236,25 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'13'!$F$2:$F$7</c:f>
+              <c:f>'13'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="2">
-                  <c:v>2.9805640124349799</c:v>
+                  <c:v>0.47429845344238097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.26148301458118</c:v>
+                  <c:v>0.100881407272675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2956195890375901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'13'!$H$2:$H$7</c:f>
+              <c:f>'13'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -259,16 +265,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.562043667287597</c:v>
+                  <c:v>43.1766535663998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.156596996786899</c:v>
+                  <c:v>21.6571527601944</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95616784071764405</c:v>
+                  <c:v>1.1733888577156899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,7 +282,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C35-493E-B596-0F62CB3DA963}"/>
+              <c16:uniqueId val="{00000000-A891-4C0A-AA93-A0735F03DB65}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -288,11 +294,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1049957567"/>
-        <c:axId val="1049959007"/>
+        <c:axId val="898283423"/>
+        <c:axId val="898289183"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1049957567"/>
+        <c:axId val="898283423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -349,12 +355,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049959007"/>
+        <c:crossAx val="898289183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1049959007"/>
+        <c:axId val="898289183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,7 +417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049957567"/>
+        <c:crossAx val="898283423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -522,7 +528,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'15'!$I$1</c:f>
+              <c:f>'15'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -553,47 +559,61 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'15'!$F$2:$F$7</c:f>
+              <c:f>'15'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>34.390505339251298</c:v>
+                  <c:v>1.5364385574572501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.514255157747101</c:v>
+                  <c:v>1.6768239255734401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9322257640588401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1111055589692098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58.262776767551102</c:v>
+                  <c:v>1.7653911789886501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'15'!$H$2:$H$7</c:f>
+              <c:f>'15'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.42592403459915501</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.6852075034425</c:v>
+                  <c:v>0.56756507410637702</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0849792289545</c:v>
+                  <c:v>12.417608085285099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5937360235842899</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36.912859552156597</c:v>
+                  <c:v>3.2092133252536899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,7 +621,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-17E8-4BC4-90C0-64D33A923A6C}"/>
+              <c16:uniqueId val="{00000000-D742-4263-BB55-203503E1982F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -613,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="749990639"/>
-        <c:axId val="840423215"/>
+        <c:axId val="1055748367"/>
+        <c:axId val="1055757007"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="749990639"/>
+        <c:axId val="1055748367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,12 +694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840423215"/>
+        <c:crossAx val="1055757007"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="840423215"/>
+        <c:axId val="1055757007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749990639"/>
+        <c:crossAx val="1055748367"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,7 +867,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3'!$I$1</c:f>
+              <c:f>'3'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -880,48 +900,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3'!$E$2:$E$7</c:f>
+              <c:f>'3'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.41422688193861201</c:v>
+                  <c:v>1.5936578839561699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32268700082854701</c:v>
+                  <c:v>1.2677951483401999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86567996287507698</c:v>
+                  <c:v>2.5572975638008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39723668915869298</c:v>
+                  <c:v>1.5402571956364199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38487369823224499</c:v>
+                  <c:v>1.4979676649140301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3'!$H$2:$H$7</c:f>
+              <c:f>'3'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.5558661720727098E-2</c:v>
+                  <c:v>7.3504151522309297E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.11332013024744E-2</c:v>
+                  <c:v>2.2090623667874398E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.73058886604297</c:v>
+                  <c:v>2.1088768075705602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33865857049369802</c:v>
+                  <c:v>0.29986232108031602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,7 +949,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DAE5-4094-B599-9B0F6CAB7BCF}"/>
+              <c16:uniqueId val="{00000000-04E0-460A-BD8E-B9C3B050900C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -941,11 +961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1043799471"/>
-        <c:axId val="1043798991"/>
+        <c:axId val="1055757487"/>
+        <c:axId val="1055750767"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1043799471"/>
+        <c:axId val="1055757487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,12 +1022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1043798991"/>
+        <c:crossAx val="1055750767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1043798991"/>
+        <c:axId val="1055750767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1084,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1043799471"/>
+        <c:crossAx val="1055757487"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1175,7 +1195,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5'!$I$1</c:f>
+              <c:f>'5'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1208,40 +1228,40 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'5'!$F$2:$F$10</c:f>
+              <c:f>'5'!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="1">
-                  <c:v>183.58876694917501</c:v>
+                  <c:v>2.2638461049630898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5389269136462</c:v>
+                  <c:v>0.18721799491019001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>162.66603244559099</c:v>
+                  <c:v>2.21129687400897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.61236663593399</c:v>
+                  <c:v>2.0237147747062201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>460.07362929256902</c:v>
+                  <c:v>2.6628273408915302</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.53100859400401</c:v>
+                  <c:v>2.0233800888523201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>286.87479906384101</c:v>
+                  <c:v>2.45769239868789</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55.534940409272103</c:v>
+                  <c:v>1.7445663101922899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5'!$H$2:$H$10</c:f>
+              <c:f>'5'!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1249,19 +1269,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.425674054587034</c:v>
+                  <c:v>0.55533520106256995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.79918461724656098</c:v>
+                  <c:v>0.95810841249484902</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58933237308338704</c:v>
+                  <c:v>0.66357904524141798</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65114613390860798</c:v>
+                  <c:v>0.58164549937857801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33165288386252301</c:v>
+                  <c:v>0.30002456976414499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,7 +1289,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4ECE-450F-8BEE-17B5B6E072D1}"/>
+              <c16:uniqueId val="{00000000-6FF7-4BBC-8760-42DB92DAE1EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1281,11 +1301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="972408735"/>
-        <c:axId val="972405855"/>
+        <c:axId val="1068959023"/>
+        <c:axId val="1068960463"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="972408735"/>
+        <c:axId val="1068959023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,12 +1362,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972405855"/>
+        <c:crossAx val="1068960463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="972405855"/>
+        <c:axId val="1068960463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1424,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="972408735"/>
+        <c:crossAx val="1068959023"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1515,7 +1535,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5a'!$I$1</c:f>
+              <c:f>'5a'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1546,55 +1566,41 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'5a'!$F$2:$F$5</c:f>
+              <c:f>'5a'!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13.0695248584331</c:v>
+                  <c:v>1.1162597991251899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6989815209433896</c:v>
+                  <c:v>0.88643327723876397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.4859257207413101</c:v>
+                  <c:v>0.97707971959916795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5a'!$H$2:$H$5</c:f>
+              <c:f>'5a'!$J$2:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.59619442027784597</c:v>
+                  <c:v>0.772252348942841</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32657792786206402</c:v>
+                  <c:v>0.33977184565730401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0342626178979999</c:v>
+                  <c:v>0.93977831967298397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1602,7 +1608,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-65A8-43E9-ACD3-55C3EA556563}"/>
+              <c16:uniqueId val="{00000000-3460-415D-871F-94EE7EDE6106}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1614,11 +1620,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="846323231"/>
-        <c:axId val="678265983"/>
+        <c:axId val="1068956623"/>
+        <c:axId val="1068973903"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="846323231"/>
+        <c:axId val="1068956623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,12 +1681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="678265983"/>
+        <c:crossAx val="1068973903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="678265983"/>
+        <c:axId val="1068973903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="846323231"/>
+        <c:crossAx val="1068956623"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1848,7 +1854,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6'!$I$1</c:f>
+              <c:f>'6'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1879,50 +1885,36 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'6'!$E$2:$E$10</c:f>
+              <c:f>'6'!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.28772677954446901</c:v>
+                  <c:v>2.20683808773562</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.2976287770757301E-2</c:v>
+                  <c:v>1.5121903600245801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4268725880109507E-2</c:v>
+                  <c:v>1.4499582859448901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18695286733230901</c:v>
+                  <c:v>1.96604947122087</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.142858205716412</c:v>
+                  <c:v>1.8159109638656199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26756115791951901</c:v>
+                  <c:v>2.1665711356348201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6'!$H$2:$H$10</c:f>
+              <c:f>'6'!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1936,19 +1928,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33341510601558799</c:v>
+                  <c:v>0.34109151672638899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38300537388112299</c:v>
+                  <c:v>0.42861234858122599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1700820436274597</c:v>
+                  <c:v>6.5088333933078397</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.1427883479316296</c:v>
+                  <c:v>7.5405072928701502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.681988691739299</c:v>
+                  <c:v>11.523434973466101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1956,7 +1948,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4FC7-4BE8-891C-C4622FCC7432}"/>
+              <c16:uniqueId val="{00000000-7876-4D47-A0B3-E36C3D53FC85}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1968,11 +1960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="840421775"/>
-        <c:axId val="840422735"/>
+        <c:axId val="1068967183"/>
+        <c:axId val="1068952303"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="840421775"/>
+        <c:axId val="1068967183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2029,12 +2021,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840422735"/>
+        <c:crossAx val="1068952303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="840422735"/>
+        <c:axId val="1068952303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2091,7 +2083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840421775"/>
+        <c:crossAx val="1068967183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2202,7 +2194,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'6a'!$I$1</c:f>
+              <c:f>'6a'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2235,22 +2227,25 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'6a'!$F$2:$F$5</c:f>
+              <c:f>'6a'!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="1">
-                  <c:v>0.37326337992833297</c:v>
+                  <c:v>-0.427984615686272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0884150388744702</c:v>
+                  <c:v>0.489735658561678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.01966151161424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6a'!$H$2:$H$5</c:f>
+              <c:f>'6a'!$J$2:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2258,13 +2253,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.36213642925469</c:v>
+                  <c:v>5.99346173557774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47263363728687002</c:v>
+                  <c:v>0.42169129089072499</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1870162654264998E-2</c:v>
+                  <c:v>2.7201304818480699E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,7 +2267,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9840-4F43-A409-CEF09DF35B1D}"/>
+              <c16:uniqueId val="{00000000-F9A6-423D-9BDF-318D3BC27BA5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2284,11 +2279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="761647343"/>
-        <c:axId val="761913983"/>
+        <c:axId val="1068974863"/>
+        <c:axId val="1068959983"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="761647343"/>
+        <c:axId val="1068974863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,12 +2340,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="761913983"/>
+        <c:crossAx val="1068959983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="761913983"/>
+        <c:axId val="1068959983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,7 +2402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="761647343"/>
+        <c:crossAx val="1068974863"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2518,7 +2513,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'7'!$I$1</c:f>
+              <c:f>'7'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2551,45 +2546,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'7'!$F$2:$F$7</c:f>
+              <c:f>'7'!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>26.1500989699855</c:v>
+                  <c:v>1.4174733368758401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60666256556119902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8626748394097299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.070620539330598</c:v>
+                  <c:v>1.54494345035321</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.5601796390159</c:v>
+                  <c:v>1.52582427682962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'7'!$H$2:$H$7</c:f>
+              <c:f>'7'!$J$2:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.24390358452308999</c:v>
+                  <c:v>0.30520205545490398</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46872140092199499</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.23444114467744401</c:v>
+                  <c:v>0.47478024802958502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0239547132744997</c:v>
+                  <c:v>3.5702893922979699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6424089665535599</c:v>
+                  <c:v>2.3742812408469902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2597,7 +2595,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-076B-4C3B-BFA5-ECCAD44E1AE0}"/>
+              <c16:uniqueId val="{00000000-4D82-4171-AF91-401BC38DF704}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2609,11 +2607,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="749953359"/>
-        <c:axId val="845488111"/>
+        <c:axId val="1068949423"/>
+        <c:axId val="1068949903"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="749953359"/>
+        <c:axId val="1068949423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2670,12 +2668,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="845488111"/>
+        <c:crossAx val="1068949903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="845488111"/>
+        <c:axId val="1068949903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2732,7 +2730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749953359"/>
+        <c:crossAx val="1068949423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2843,7 +2841,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'9'!$I$1</c:f>
+              <c:f>'9'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2874,50 +2872,67 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'9'!$F$2:$F$8</c:f>
+              <c:f>'9'!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>165.823972739732</c:v>
+                  <c:v>2.21964731557483</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.054074208547597</c:v>
+                  <c:v>1.55695434828742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.6815348320814</c:v>
+                  <c:v>1.5008062130991799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134.504322807786</c:v>
+                  <c:v>2.1287362422670499</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.617676426121797</c:v>
+                  <c:v>1.78970531724707</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88.194470217674905</c:v>
+                  <c:v>1.94544135577539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'9'!$H$2:$H$8</c:f>
+              <c:f>'9'!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.3297639505519001</c:v>
+                  <c:v>1.82328254299512</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21060279927259001</c:v>
+                  <c:v>0.26097334154129898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2231410310497299</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.488676963637731</c:v>
+                  <c:v>0.43358295603590602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2925,7 +2940,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EF9B-43B6-8C5B-5548F33B4184}"/>
+              <c16:uniqueId val="{00000000-FF89-4223-95F6-CFFA2A2A46CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2937,11 +2952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="758572239"/>
-        <c:axId val="758570319"/>
+        <c:axId val="1068971983"/>
+        <c:axId val="1068945583"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="758572239"/>
+        <c:axId val="1068971983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,12 +3013,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="758570319"/>
+        <c:crossAx val="1068945583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="758570319"/>
+        <c:axId val="1068945583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,7 +3075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="758572239"/>
+        <c:crossAx val="1068971983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8124,23 +8139,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B84C845F-5D3A-2E69-5F6B-73346B00E2A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D289C21B-24CB-73C1-B476-5F3377F28F83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8165,23 +8180,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07ACEED-5D52-F97A-ED62-D2D73B88983F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DB0941-1CF5-2B80-53D2-BBD8160F4A7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8206,23 +8221,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64501E84-D922-5B2F-C596-24A226E20AC0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC2FEAF-0271-270E-9A9F-2B501A1C4A7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8247,23 +8262,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB96335E-8657-E5A8-D0FD-1A735FF774D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{179CEEF1-184F-B7B7-CC12-9A624DA1F36C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8288,23 +8303,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3C466D-C54B-F61A-8F93-09FF6CBB58FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8313FFAD-BC7A-EE81-D8AC-FF9CF21A7306}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8329,23 +8344,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>633412</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>633412</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F6F5BF0-43E8-074F-85A8-B32BCC1EE300}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127969F6-C59D-5B2F-ECF5-72B73A478DEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8370,23 +8385,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2729A135-F053-DF5F-8137-A829553A3FE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B39EF9A-B8D0-B260-66B7-5A75FB2BCA0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8411,23 +8426,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4260EF00-EA0F-735C-3670-1B0515B23FCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C0CAF1D-E15A-F5B6-464B-8D1F714C959C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8452,23 +8467,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA947931-7250-342F-CA57-2996235ED2DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{106ED7FA-840E-8325-B5BC-7BA5B1C4B065}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8768,15 +8783,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8796,55 +8811,58 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45442</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>737.67287999999996</v>
       </c>
-      <c r="H2" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I2" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J2" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45590</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>365.64864</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45331</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>609.13812959999996</v>
@@ -8859,38 +8877,41 @@
         <v>2.9805640124349799</v>
       </c>
       <c r="G4">
+        <v>0.47429845344238097</v>
+      </c>
+      <c r="H4">
         <v>58.711833333333303</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>35.562043667287597</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>43.1766535663998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45569</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>410.61864000000003</v>
       </c>
-      <c r="H5" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I5" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J5" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45231</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>840.86069999999995</v>
@@ -8905,21 +8926,24 @@
         <v>1.26148301458118</v>
       </c>
       <c r="G6">
+        <v>0.100881407272675</v>
+      </c>
+      <c r="H6">
         <v>68.241833333333304</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>21.156596996786899</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>21.6571527601944</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45279</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>654.34670000000006</v>
@@ -8930,11 +8954,20 @@
       <c r="E7">
         <v>0.33558506980650299</v>
       </c>
+      <c r="F7">
+        <v>197.52387140350299</v>
+      </c>
       <c r="G7">
+        <v>2.2956195890375901</v>
+      </c>
+      <c r="H7">
         <v>58.136791666666703</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.95616784071764405</v>
+      </c>
+      <c r="J7">
+        <v>1.1733888577156899</v>
       </c>
     </row>
   </sheetData>
@@ -8946,15 +8979,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8974,21 +9007,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>655.34429999999998</v>
@@ -9003,21 +9039,24 @@
         <v>34.390505339251298</v>
       </c>
       <c r="G2">
+        <v>1.5364385574572501</v>
+      </c>
+      <c r="H2">
         <v>53.767708333333303</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.42592403459915501</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.56756507410637702</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45484</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>779.41542000000004</v>
@@ -9032,38 +9071,38 @@
         <v>47.514255157747101</v>
       </c>
       <c r="G3">
+        <v>1.6768239255734401</v>
+      </c>
+      <c r="H3">
         <v>76.441249999999997</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>15.6852075034425</v>
       </c>
-      <c r="I3">
-        <v>13.9945930170877</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45590</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>532.55862000000002</v>
       </c>
-      <c r="H4" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I4" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J4" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45279</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>699.4171</v>
@@ -9074,19 +9113,28 @@
       <c r="E5">
         <v>0.52826006985347296</v>
       </c>
+      <c r="F5">
+        <v>855.51132713685695</v>
+      </c>
       <c r="G5">
+        <v>2.9322257640588401</v>
+      </c>
+      <c r="H5">
         <v>57.950125</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>10.0849792289545</v>
       </c>
+      <c r="J5">
+        <v>12.417608085285099</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45502</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>801.76949999999999</v>
@@ -9097,19 +9145,28 @@
       <c r="E6">
         <v>0.31201786247728303</v>
       </c>
+      <c r="F6">
+        <v>129.15331535889499</v>
+      </c>
       <c r="G6">
+        <v>2.1111055589692098</v>
+      </c>
+      <c r="H6">
         <v>76.383166666666696</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>3.5937360235842899</v>
       </c>
+      <c r="J6">
+        <v>3.2092133252536899</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45569</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>547.61717999999996</v>
@@ -9124,13 +9181,13 @@
         <v>58.262776767551102</v>
       </c>
       <c r="G7">
+        <v>1.7653911789886501</v>
+      </c>
+      <c r="H7">
         <v>76.3036666666667</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>36.912859552156597</v>
-      </c>
-      <c r="I7">
-        <v>33.0116836786571</v>
       </c>
     </row>
   </sheetData>
@@ -9142,15 +9199,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9170,21 +9227,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>473.84879999999998</v>
@@ -9199,38 +9259,41 @@
         <v>39.2335750636623</v>
       </c>
       <c r="G2">
+        <v>1.5936578839561699</v>
+      </c>
+      <c r="H2">
         <v>54.145791666666703</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>5.5558661720727098E-2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>7.3504151522309297E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45590</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>411.06707999999998</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45231</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>730.71659999999997</v>
@@ -9245,21 +9308,24 @@
         <v>18.5265754025319</v>
       </c>
       <c r="G4">
+        <v>1.2677951483401999</v>
+      </c>
+      <c r="H4">
         <v>67.036416666666696</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2.11332013024744E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2.2090623667874398E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45279</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>699.4171</v>
@@ -9274,21 +9340,24 @@
         <v>360.82578389464197</v>
       </c>
       <c r="G5">
+        <v>2.5572975638008</v>
+      </c>
+      <c r="H5">
         <v>58.517166666666697</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.73058886604297</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2.1088768075705602</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45505</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>752.10996</v>
@@ -9303,21 +9372,24 @@
         <v>34.6942253975892</v>
       </c>
       <c r="G6">
+        <v>1.5402571956364199</v>
+      </c>
+      <c r="H6">
         <v>76.912333333333294</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.33865857049369802</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.29986232108031602</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45569</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>395.73576000000003</v>
@@ -9332,7 +9404,13 @@
         <v>31.475139594695701</v>
       </c>
       <c r="G7">
+        <v>1.4979676649140301</v>
+      </c>
+      <c r="H7">
         <v>75.441000000000003</v>
+      </c>
+      <c r="I7">
+        <v>6.3222902982053197</v>
       </c>
     </row>
   </sheetData>
@@ -9344,15 +9422,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9372,38 +9450,41 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45442</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>688.71222</v>
       </c>
-      <c r="H2" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I2" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J2" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45484</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>690.81389999999999</v>
@@ -9418,15 +9499,21 @@
         <v>183.58876694917501</v>
       </c>
       <c r="G3">
+        <v>2.2638461049630898</v>
+      </c>
+      <c r="H3">
         <v>76.579041666666697</v>
       </c>
+      <c r="I3">
+        <v>4.7455135401012898</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45590</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>548.14409999999998</v>
@@ -9441,15 +9528,21 @@
         <v>1.5389269136462</v>
       </c>
       <c r="G4">
+        <v>0.18721799491019001</v>
+      </c>
+      <c r="H4">
         <v>69.716999999999999</v>
       </c>
+      <c r="I4">
+        <v>47.996062389961097</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45296</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>429.05880000000002</v>
@@ -9464,21 +9557,24 @@
         <v>162.66603244559099</v>
       </c>
       <c r="G5">
+        <v>2.21129687400897</v>
+      </c>
+      <c r="H5">
         <v>54.871041666666699</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.425674054587034</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.55533520106256995</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45266</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>409.7124</v>
@@ -9493,15 +9589,21 @@
         <v>105.61236663593399</v>
       </c>
       <c r="G6">
+        <v>2.0237147747062201</v>
+      </c>
+      <c r="H6">
         <v>62.968666666666699</v>
       </c>
+      <c r="I6">
+        <v>1.9954189154176001</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45279</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>444.28</v>
@@ -9516,21 +9618,24 @@
         <v>460.07362929256902</v>
       </c>
       <c r="G7">
+        <v>2.6628273408915302</v>
+      </c>
+      <c r="H7">
         <v>59.392708333333303</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.79918461724656098</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.95810841249484902</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45376</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>545.70809999999994</v>
@@ -9545,21 +9650,24 @@
         <v>105.53100859400401</v>
       </c>
       <c r="G8">
+        <v>2.0233800888523201</v>
+      </c>
+      <c r="H8">
         <v>62.832791666666701</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.58933237308338704</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.66357904524141798</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45502</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>776.96429999999998</v>
@@ -9574,21 +9682,24 @@
         <v>286.87479906384101</v>
       </c>
       <c r="G9">
+        <v>2.45769239868789</v>
+      </c>
+      <c r="H9">
         <v>76.361791666666704</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.65114613390860798</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.58164549937857801</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45569</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>395.84652</v>
@@ -9603,12 +9714,15 @@
         <v>55.534940409272103</v>
       </c>
       <c r="G10">
+        <v>1.7445663101922899</v>
+      </c>
+      <c r="H10">
         <v>75.600666666666697</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.33165288386252301</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.30002456976414499</v>
       </c>
     </row>
@@ -9621,15 +9735,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" activeCellId="1" sqref="F1:F1048576 I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9649,21 +9763,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>650.67600000000004</v>
@@ -9678,38 +9795,41 @@
         <v>13.0695248584331</v>
       </c>
       <c r="G2">
+        <v>1.1162597991251899</v>
+      </c>
+      <c r="H2">
         <v>55.262291666666698</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.59619442027784597</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.772252348942841</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45590</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>835.77359999999999</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45231</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>402.31270000000001</v>
@@ -9724,21 +9844,24 @@
         <v>7.6989815209433896</v>
       </c>
       <c r="G4">
+        <v>0.88643327723876397</v>
+      </c>
+      <c r="H4">
         <v>67.299833333333297</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.32657792786206402</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.33977184565730401</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45569</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>547.30542000000003</v>
@@ -9753,12 +9876,15 @@
         <v>9.4859257207413101</v>
       </c>
       <c r="G5">
+        <v>0.97707971959916795</v>
+      </c>
+      <c r="H5">
         <v>75.319166666666703</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.0342626178979999</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.93977831967298397</v>
       </c>
     </row>
@@ -9771,15 +9897,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9799,21 +9925,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>644.81269999999995</v>
@@ -9828,66 +9957,72 @@
         <v>161.004527140063</v>
       </c>
       <c r="G2">
+        <v>2.20683808773562</v>
+      </c>
+      <c r="H2">
         <v>57.347416666666703</v>
       </c>
+      <c r="I2">
+        <v>203.66771770116301</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45442</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>645.07506000000001</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45484</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>20605.830000000002</v>
       </c>
-      <c r="H4" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I4" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J4" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45590</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>502.29234000000002</v>
       </c>
-      <c r="H5" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I5" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J5" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45231</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>698.6585</v>
@@ -9902,21 +10037,24 @@
         <v>32.522982093317097</v>
       </c>
       <c r="G6">
+        <v>1.5121903600245801</v>
+      </c>
+      <c r="H6">
         <v>68.278565217391304</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.33341510601558799</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.34109151672638899</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45266</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>595.43700000000001</v>
@@ -9931,21 +10069,24 @@
         <v>28.181122381291299</v>
       </c>
       <c r="G7">
+        <v>1.4499582859448901</v>
+      </c>
+      <c r="H7">
         <v>63.182749999999999</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.38300537388112299</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.42861234858122599</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45331</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>433.461546</v>
@@ -9960,21 +10101,24 @@
         <v>92.480351387484305</v>
       </c>
       <c r="G8">
+        <v>1.96604947122087</v>
+      </c>
+      <c r="H8">
         <v>56.771625</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>5.1700820436274597</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6.5088333933078397</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45502</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>667.35563999999999</v>
@@ -9989,21 +10133,24 @@
         <v>65.450197871718402</v>
       </c>
       <c r="G9">
+        <v>1.8159109638656199</v>
+      </c>
+      <c r="H9">
         <v>74.173434782608695</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>8.1427883479316296</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>7.5405072928701502</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45569</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>395.63819999999998</v>
@@ -10018,12 +10165,15 @@
         <v>146.747643377652</v>
       </c>
       <c r="G10">
+        <v>2.1665711356348201</v>
+      </c>
+      <c r="H10">
         <v>75.326458333333306</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>12.681988691739299</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>11.523434973466101</v>
       </c>
     </row>
@@ -10036,15 +10186,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10064,38 +10214,44 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45590</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>411.13853999999998</v>
       </c>
-      <c r="H2" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I2" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J2" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45296</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>637.03409999999997</v>
@@ -10110,21 +10266,27 @@
         <v>0.37326337992833297</v>
       </c>
       <c r="G3">
+        <v>-0.427984615686272</v>
+      </c>
+      <c r="H3">
         <v>52.158749999999998</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>4.36213642925469</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.99346173557774</v>
       </c>
+      <c r="K3">
+        <v>-0.427984615686272</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45502</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>647.25275999999997</v>
@@ -10139,21 +10301,27 @@
         <v>3.0884150388744702</v>
       </c>
       <c r="G4">
+        <v>0.489735658561678</v>
+      </c>
+      <c r="H4">
         <v>76.433750000000003</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.47263363728687002</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.42169129089072499</v>
       </c>
+      <c r="K4">
+        <v>0.489735658561678</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45279</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>801.09990000000005</v>
@@ -10164,11 +10332,23 @@
       <c r="E5">
         <v>0.38613206590049598</v>
       </c>
+      <c r="F5">
+        <v>104.63127357915801</v>
+      </c>
       <c r="G5">
+        <v>2.01966151161424</v>
+      </c>
+      <c r="H5">
         <v>57.410541666666703</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2.1870162654264998E-2</v>
+      </c>
+      <c r="J5">
+        <v>2.7201304818480699E-2</v>
+      </c>
+      <c r="K5">
+        <v>2.01966151161424</v>
       </c>
     </row>
   </sheetData>
@@ -10180,15 +10360,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10208,21 +10388,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>679.72839999999997</v>
@@ -10237,38 +10420,41 @@
         <v>26.1500989699855</v>
       </c>
       <c r="G2">
+        <v>1.4174733368758401</v>
+      </c>
+      <c r="H2">
         <v>57.088374999999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.24390358452308999</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.30520205545490398</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45590</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>441.74369999999999</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45231</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>719.91600000000005</v>
@@ -10279,19 +10465,28 @@
       <c r="E4">
         <v>0.13055244711888001</v>
       </c>
+      <c r="F4">
+        <v>4.0426166984303</v>
+      </c>
       <c r="G4">
+        <v>0.60666256556119902</v>
+      </c>
+      <c r="H4">
         <v>68.842375000000004</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.46872140092199499</v>
       </c>
+      <c r="J4">
+        <v>0.47478024802958502</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45279</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>418.92230000000001</v>
@@ -10302,22 +10497,25 @@
       <c r="E5">
         <v>0.73138680186451299</v>
       </c>
+      <c r="F5">
+        <v>728.91156257831699</v>
+      </c>
       <c r="G5">
+        <v>2.8626748394097299</v>
+      </c>
+      <c r="H5">
         <v>60.173708333333302</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.23444114467744401</v>
       </c>
-      <c r="I5">
-        <v>0.27708508441848401</v>
-      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45505</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>642.23753999999997</v>
@@ -10332,21 +10530,24 @@
         <v>35.070620539330598</v>
       </c>
       <c r="G6">
+        <v>1.54494345035321</v>
+      </c>
+      <c r="H6">
         <v>76.782291666666694</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4.0239547132744997</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3.5702893922979699</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45569</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>365.72465999999997</v>
@@ -10361,12 +10562,15 @@
         <v>33.5601796390159</v>
       </c>
       <c r="G7">
+        <v>1.52582427682962</v>
+      </c>
+      <c r="H7">
         <v>76.006291666666698</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2.6424089665535599</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2.3742812408469902</v>
       </c>
     </row>
@@ -10379,15 +10583,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10407,21 +10611,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45296</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>699.58140000000003</v>
@@ -10436,38 +10643,41 @@
         <v>165.823972739732</v>
       </c>
       <c r="G2">
+        <v>2.21964731557483</v>
+      </c>
+      <c r="H2">
         <v>52.267458333333302</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.3297639505519001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1.82328254299512</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45590</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>380.19384000000002</v>
       </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
       <c r="I3" t="e">
         <v>#NUM!</v>
       </c>
+      <c r="J3" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45231</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>721.23059999999998</v>
@@ -10482,15 +10692,21 @@
         <v>36.054074208547597</v>
       </c>
       <c r="G4">
+        <v>1.55695434828742</v>
+      </c>
+      <c r="H4">
         <v>65.837708333333296</v>
       </c>
+      <c r="I4">
+        <v>1.82495889091172</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45266</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>739.46839999999997</v>
@@ -10505,21 +10721,24 @@
         <v>31.6815348320814</v>
       </c>
       <c r="G5">
+        <v>1.5008062130991799</v>
+      </c>
+      <c r="H5">
         <v>57.605125000000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.21060279927259001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.26097334154129898</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45331</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>447.77111400000001</v>
@@ -10534,15 +10753,21 @@
         <v>134.504322807786</v>
       </c>
       <c r="G6">
+        <v>2.1287362422670499</v>
+      </c>
+      <c r="H6">
         <v>55.680374999999998</v>
       </c>
+      <c r="I6">
+        <v>36.698976971219601</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45502</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>719.93502000000001</v>
@@ -10557,15 +10782,24 @@
         <v>61.617676426121797</v>
       </c>
       <c r="G7">
+        <v>1.78970531724707</v>
+      </c>
+      <c r="H7">
         <v>77.678708333333304</v>
       </c>
+      <c r="I7">
+        <v>2.54253644329191</v>
+      </c>
+      <c r="J7">
+        <v>2.2231410310497299</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45569</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>396.4812</v>
@@ -10580,12 +10814,15 @@
         <v>88.194470217674905</v>
       </c>
       <c r="G8">
+        <v>1.94544135577539</v>
+      </c>
+      <c r="H8">
         <v>76.782666666666699</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.488676963637731</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.43358295603590602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code for K600 and stream metabolism
</commit_message>
<xml_diff>
--- a/04_Output/rC_k600_edited.xlsx
+++ b/04_Output/rC_k600_edited.xlsx
@@ -8,29 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\04_Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98BA9D9-6732-4078-A2FD-E962ACADBDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4F5157-8968-46A8-86BA-FC6CF7258591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="10070" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="10" windowWidth="19095" windowHeight="10070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
-    <sheet name="15" sheetId="3" r:id="rId2"/>
-    <sheet name="3" sheetId="4" r:id="rId3"/>
-    <sheet name="5" sheetId="5" r:id="rId4"/>
-    <sheet name="5a" sheetId="6" r:id="rId5"/>
-    <sheet name="6" sheetId="7" r:id="rId6"/>
-    <sheet name="6a" sheetId="8" r:id="rId7"/>
-    <sheet name="7" sheetId="9" r:id="rId8"/>
-    <sheet name="9" sheetId="10" r:id="rId9"/>
+    <sheet name="15" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
+    <sheet name="5" sheetId="4" r:id="rId4"/>
+    <sheet name="5a" sheetId="5" r:id="rId5"/>
+    <sheet name="6" sheetId="6" r:id="rId6"/>
+    <sheet name="6a" sheetId="7" r:id="rId7"/>
+    <sheet name="7" sheetId="8" r:id="rId8"/>
+    <sheet name="9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="20">
   <si>
-    <t>day</t>
+    <t>logQ</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>ID</t>
@@ -57,7 +60,7 @@
     <t>k600_1d</t>
   </si>
   <si>
-    <t>logQ</t>
+    <t>log_K600</t>
   </si>
   <si>
     <t>13</t>
@@ -92,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -201,8 +204,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'13'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -223,47 +237,52 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'13'!$E$2:$E$7</c:f>
+              <c:f>'13'!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.47429845344238097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.100881407272675</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3458550098918499E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.67414206545583E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.33558506980650299</c:v>
+                  <c:v>2.2956195890375901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'13'!$I$2:$I$7</c:f>
+              <c:f>'13'!$K$2:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.4720682359536399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.19247311371887</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.1766535663998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.9458937661225804</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1733888577156899</c:v>
+                  <c:v>0.47387400561080101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -271,7 +290,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-741B-4804-93DD-D9286BABFDEB}"/>
+              <c16:uniqueId val="{00000000-4367-4226-B2CE-D6F83FC215CE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -283,11 +302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1548816031"/>
-        <c:axId val="1548817471"/>
+        <c:axId val="1452312607"/>
+        <c:axId val="1452313087"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1548816031"/>
+        <c:axId val="1452312607"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -344,12 +363,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1548817471"/>
+        <c:crossAx val="1452313087"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1548817471"/>
+        <c:axId val="1452313087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1548816031"/>
+        <c:crossAx val="1452312607"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -508,17 +527,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.6580927384076991E-2"/>
-          <c:y val="0.17171296296296298"/>
-          <c:w val="0.88386351706036748"/>
-          <c:h val="0.72088764946048411"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -527,11 +536,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'15'!$I$1</c:f>
+              <c:f>'15'!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k600_1d</c:v>
+                  <c:v>log_K600</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -560,54 +569,51 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'15'!$E$2:$E$7</c:f>
+              <c:f>'15'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.215852248068133</c:v>
+                  <c:v>1.5364385574572501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23609790544256401</c:v>
+                  <c:v>1.6768239255734401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16324969531057901</c:v>
+                  <c:v>1.1028312072387401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52826006985347296</c:v>
+                  <c:v>2.9322257640588401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31201786247728303</c:v>
+                  <c:v>2.1111055589692098</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24996315545078601</c:v>
+                  <c:v>1.7653911789886501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'15'!$I$2:$I$7</c:f>
+              <c:f>'15'!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.56756507410637702</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.9945930170877</c:v>
+                  <c:v>1.52962388841246</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.9019208028636</c:v>
+                  <c:v>2.1261592525806399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.417608085285099</c:v>
+                  <c:v>1.48120094839522</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.7553315960599</c:v>
+                  <c:v>1.97991814613576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.0116836786571</c:v>
+                  <c:v>2.3699845090321801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,7 +621,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-41F3-4348-82E3-78DBD9C3D429}"/>
+              <c16:uniqueId val="{00000000-FF8C-4C0F-9996-4425D376B47F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -627,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147369391"/>
-        <c:axId val="147370831"/>
+        <c:axId val="1660840591"/>
+        <c:axId val="1452299167"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147369391"/>
+        <c:axId val="1660840591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,12 +694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147370831"/>
+        <c:crossAx val="1452299167"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147370831"/>
+        <c:axId val="1452299167"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147369391"/>
+        <c:crossAx val="1660840591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -821,14 +827,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.56782633420822393"/>
-          <c:y val="2.7898874269439419E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -860,15 +858,36 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.0539370078740152E-2"/>
+          <c:y val="0.16708333333333336"/>
+          <c:w val="0.8825717410323709"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -891,51 +910,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3'!$E$2:$E$7</c:f>
+              <c:f>'3'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.41422688193861201</c:v>
+                  <c:v>1.5901312641124601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35358594626280099</c:v>
+                  <c:v>1.3870902571252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32268700082854701</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.86567996287507698</c:v>
+                  <c:v>1.2690811021975701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39723668915869298</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.38487369823224499</c:v>
+                  <c:v>1.4983746072415201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3'!$I$2:$I$7</c:f>
+              <c:f>'3'!$K$2:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.3504151522309297E-2</c:v>
+                  <c:v>-1.0336055520613401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31419620586510399</c:v>
+                  <c:v>0.33046359994212099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2090623667874398E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1088768075705602</c:v>
+                  <c:v>-1.1198634405211101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29986232108031602</c:v>
+                  <c:v>1.12727027775397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -943,7 +953,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-68CC-4B5E-9936-0967286338BC}"/>
+              <c16:uniqueId val="{00000000-BFFC-4A28-9A71-0FBE058ECBA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -955,11 +965,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1207103871"/>
-        <c:axId val="1207106751"/>
+        <c:axId val="656774592"/>
+        <c:axId val="656780352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1207103871"/>
+        <c:axId val="656774592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,12 +1026,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1207106751"/>
+        <c:crossAx val="656780352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1207106751"/>
+        <c:axId val="656780352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1207103871"/>
+        <c:crossAx val="656774592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1187,8 +1197,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1209,34 +1230,42 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'5'!$J$2:$J$11</c:f>
+              <c:f>'5'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="1">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
                   <c:v>2.2638461049630898</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.21129687400897</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18721799491019001</c:v>
+                  <c:v>2.0237147747062201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6628273408915302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.21129687400897</c:v>
+                  <c:v>2.45769239868789</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0237147747062201</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.6628273408915302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.0233800888523201</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.45769239868789</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>1.7445663101922899</c:v>
                 </c:pt>
               </c:numCache>
@@ -1244,36 +1273,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5'!$I$2:$I$11</c:f>
+              <c:f>'5'!$K$2:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.668476072734428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2240976016608602</c:v>
+                  <c:v>0.77854869405477301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81087624729699004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.36288571204037201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55533520106256995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2417182470070598</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.95810841249484902</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.66357904524141798</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.58164549937857801</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.30002456976414499</c:v>
+                  <c:v>0.130357159032578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1281,7 +1298,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E415-48C2-AFF2-E9DBD812E96B}"/>
+              <c16:uniqueId val="{00000000-5C4A-49F4-82FF-2314A56BD659}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1293,11 +1310,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1706706079"/>
-        <c:axId val="1706703199"/>
+        <c:axId val="1594994287"/>
+        <c:axId val="1666648751"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1706706079"/>
+        <c:axId val="1594994287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1354,12 +1371,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1706703199"/>
+        <c:crossAx val="1666648751"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1706703199"/>
+        <c:axId val="1666648751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1706706079"/>
+        <c:crossAx val="1594994287"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1525,8 +1542,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5a'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1549,7 +1577,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'5a'!$J$2:$J$5</c:f>
+              <c:f>'5a'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1570,21 +1598,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5a'!$I$2:$I$5</c:f>
+              <c:f>'5a'!$K$2:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.772252348942841</c:v>
+                  <c:v>0.275765685014141</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.22687990873807</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33977184565730401</c:v>
+                  <c:v>1.6422222231553301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.93977831967298397</c:v>
+                  <c:v>0.85258190192095995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1592,7 +1617,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4655-4F94-99BC-9B076D6511C3}"/>
+              <c16:uniqueId val="{00000000-513F-4586-9D8E-27EDF04981B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1604,11 +1629,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64709231"/>
-        <c:axId val="64706351"/>
+        <c:axId val="1666637231"/>
+        <c:axId val="1666644431"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64709231"/>
+        <c:axId val="1666637231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1665,12 +1690,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64706351"/>
+        <c:crossAx val="1666644431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64706351"/>
+        <c:axId val="1666644431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64709231"/>
+        <c:crossAx val="1666637231"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1836,8 +1861,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'6'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1858,34 +1894,48 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'6'!$J$2:$J$11</c:f>
+              <c:f>'6'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2.20683808773562</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="1">
                   <c:v>2.0309945857151401</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="2">
                   <c:v>1.8044538113953601</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1421668183018401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4499582859448901</c:v>
+                </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5121903600245801</c:v>
+                  <c:v>1.96604947122087</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4499582859448901</c:v>
+                  <c:v>1.8159109638656199</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.96604947122087</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.8159109638656199</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>2.1665711356348201</c:v>
                 </c:pt>
               </c:numCache>
@@ -1893,33 +1943,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6'!$I$2:$I$11</c:f>
+              <c:f>'6'!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.1610877322831099</c:v>
+                  <c:v>0.45660363252434699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.46730739347396</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.12293103678092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0365221508306601</c:v>
+                  <c:v>2.5673865013158799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34109151672638899</c:v>
+                  <c:v>1.10532903433306</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42861234858122599</c:v>
+                  <c:v>1.6450230509194299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5088333933078397</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.93487253220809396</c:v>
+                  <c:v>0.51532489814205995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,7 +1974,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F848-48BF-BB03-D2BF6B79784A}"/>
+              <c16:uniqueId val="{00000000-CDC2-416B-A158-81B77391BDE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1939,11 +1986,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152015151"/>
-        <c:axId val="64707791"/>
+        <c:axId val="1666636271"/>
+        <c:axId val="1666658831"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152015151"/>
+        <c:axId val="1666636271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,12 +2047,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64707791"/>
+        <c:crossAx val="1666658831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64707791"/>
+        <c:axId val="1666658831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,7 +2109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152015151"/>
+        <c:crossAx val="1666636271"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2171,8 +2218,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'6a'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2193,16 +2251,36 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'6a'!$J$4:$J$5</c:f>
+              <c:f>'6a'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>-0.70444482698631605</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.427984615686272</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.489735658561678</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>2.01966151161424</c:v>
                 </c:pt>
               </c:numCache>
@@ -2210,15 +2288,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'6a'!$I$4:$I$5</c:f>
+              <c:f>'6a'!$K$2:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.42169129089072499</c:v>
+                  <c:v>2.3224106793333701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7201304818480699E-2</c:v>
+                  <c:v>1.1238182847190901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49886052133811898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.93371932197318797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,7 +2310,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E4D2-4A0C-BDC1-2F9A19C94941}"/>
+              <c16:uniqueId val="{00000000-7A7D-4CE3-821E-3DB0F37F1119}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2238,11 +2322,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1706827247"/>
-        <c:axId val="1706828207"/>
+        <c:axId val="1666663631"/>
+        <c:axId val="1666661231"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1706827247"/>
+        <c:axId val="1666663631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,12 +2383,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1706828207"/>
+        <c:crossAx val="1666661231"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1706828207"/>
+        <c:axId val="1666661231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2361,7 +2445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1706827247"/>
+        <c:crossAx val="1666663631"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2470,8 +2554,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'7'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2494,10 +2589,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'7'!$J$2:$J$7</c:f>
+              <c:f>'7'!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1.4174733368758401</c:v>
                 </c:pt>
@@ -2511,9 +2606,6 @@
                   <c:v>2.8626748394097299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.54494345035321</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1.52582427682962</c:v>
                 </c:pt>
               </c:numCache>
@@ -2521,27 +2613,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'7'!$I$2:$I$7</c:f>
+              <c:f>'7'!$K$2:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.30520205545490398</c:v>
+                  <c:v>0.34046807582660699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.99799058223319</c:v>
+                  <c:v>0.88678515178480999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47478024802958502</c:v>
+                  <c:v>0.57113352431083098</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27708508441848401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.5702893922979699</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3742812408469902</c:v>
+                  <c:v>-0.15928632428432901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2549,7 +2635,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-00A9-4D50-B012-198707371CD9}"/>
+              <c16:uniqueId val="{00000000-DF21-4B0C-9D22-2B89C64B5268}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2561,11 +2647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1115115967"/>
-        <c:axId val="57939583"/>
+        <c:axId val="1661088671"/>
+        <c:axId val="1661088191"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1115115967"/>
+        <c:axId val="1661088671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2622,12 +2708,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57939583"/>
+        <c:crossAx val="1661088191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57939583"/>
+        <c:axId val="1661088191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,7 +2770,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1115115967"/>
+        <c:crossAx val="1661088671"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2786,25 +2872,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.2692038495188102E-2"/>
-          <c:y val="0.19486111111111112"/>
-          <c:w val="0.88704418197725288"/>
-          <c:h val="0.72088764946048411"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'9'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_K600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2827,7 +2914,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'9'!$J$2:$J$9</c:f>
+              <c:f>'9'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2841,7 +2928,7 @@
                   <c:v>1.7498332898101401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.55695434828742</c:v>
+                  <c:v>1.41438658720066</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.5008062130991799</c:v>
@@ -2860,24 +2947,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'9'!$I$2:$I$9</c:f>
+              <c:f>'9'!$K$2:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.82328254299512</c:v>
+                  <c:v>0.64794522995038195</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9477536276551799</c:v>
+                <c:pt idx="1">
+                  <c:v>0.36575537475554798</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.26097334154129898</c:v>
+                <c:pt idx="2">
+                  <c:v>0.78359871795927805</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2231410310497299</c:v>
+                  <c:v>1.2073581606603301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43358295603590602</c:v>
+                  <c:v>0.49568526267976798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2885,7 +2972,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7A20-447B-817F-929B5F2997BC}"/>
+              <c16:uniqueId val="{00000000-6446-4082-96AC-804B3FDD3254}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2897,11 +2984,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1352187631"/>
-        <c:axId val="1200346191"/>
+        <c:axId val="654426720"/>
+        <c:axId val="654426240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1352187631"/>
+        <c:axId val="654426720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2958,12 +3045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1200346191"/>
+        <c:crossAx val="654426240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1200346191"/>
+        <c:axId val="654426240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3020,7 +3107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1352187631"/>
+        <c:crossAx val="654426720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8084,23 +8171,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>334962</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>39007</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>334962</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>159657</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12B9B65-B5CD-C0F1-E235-FDF4939082CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FACEF18-7CAD-8B4A-1CAD-0CFFC3468D12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8125,23 +8212,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>11112</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11112</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6997D22E-B54A-CF6C-7341-28CB6E1F5AFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2CF58A4-FC84-5703-806B-FA3FC56D86B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8166,23 +8253,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>592930</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>42070</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>592930</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16818CB-81E2-F1C3-4167-B37BCAFA6D96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69937280-4E9A-78CF-9685-D9CB385D6F98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8207,23 +8294,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>544512</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>544512</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A516B4-A732-8EBD-E230-4920E7FF1F88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D16480-95EB-30E7-821A-215637D84512}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8248,23 +8335,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>668337</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>46037</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>668337</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>46037</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D973A02-9C69-481B-8E3B-452E5B386C2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD954EF3-8186-5186-A6EF-1636373915FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8289,23 +8376,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>46037</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>46037</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26D64D33-AD73-F614-0BD5-2B226587D0DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DEFB90-887B-27B9-65AA-8CFBE62DE0E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8330,23 +8417,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E5C96D-36CD-08F2-7627-D2487D9394F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1BE5C9-8856-0082-A461-D50A9A57B909}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8371,23 +8458,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>204787</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>204787</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6392EC2B-0DED-F19B-7A60-564B55BC754F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEECE9C2-6001-4309-BF7E-5BEF1AA70642}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8412,23 +8499,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>503237</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>503237</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12685800-BBDC-90BA-C0A1-F8EFB51BC511}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15880E42-38B9-A88F-B5F8-C541BA36B06B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8728,15 +8815,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8767,152 +8854,113 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45442</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>737.67287999999996</v>
-      </c>
-      <c r="H2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I2" t="e">
-        <v>#NUM!</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>0.47429845344238097</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45331.546296296299</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>841.73281919999999</v>
+      </c>
+      <c r="E2">
+        <v>2525.2719999999999</v>
+      </c>
+      <c r="F2">
+        <v>5.3458550098918499E-2</v>
+      </c>
+      <c r="G2">
+        <v>2.9805640124349799</v>
+      </c>
+      <c r="H2">
+        <v>58.711833333333303</v>
+      </c>
+      <c r="I2">
+        <v>2442.33913134876</v>
+      </c>
+      <c r="J2">
+        <v>2965.2972577307</v>
+      </c>
+      <c r="K2">
+        <v>3.4720682359536399</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>365.64864</v>
-      </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#NUM!</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>0.100881407272675</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45231.643750000003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>861.60841666666704</v>
+      </c>
+      <c r="E3">
+        <v>4695.2049999999999</v>
+      </c>
+      <c r="F3">
+        <v>3.67414206545583E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.26148301458118</v>
+      </c>
+      <c r="H3">
+        <v>68.241833333333304</v>
+      </c>
+      <c r="I3">
+        <v>15.2165979978598</v>
+      </c>
+      <c r="J3">
+        <v>15.5766160020993</v>
+      </c>
+      <c r="K3">
+        <v>1.19247311371887</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45331</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>609.13812959999996</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>2.2956195890375901</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45279.638888888898</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>2525.2719999999999</v>
+        <v>682.46505000000002</v>
       </c>
       <c r="E4">
-        <v>5.3458550098918499E-2</v>
+        <v>4360.4979999999996</v>
       </c>
       <c r="F4">
-        <v>2.9805640124349799</v>
+        <v>0.33558506980650299</v>
       </c>
       <c r="G4">
-        <v>58.711833333333303</v>
+        <v>197.52387140350299</v>
       </c>
       <c r="H4">
-        <v>35.562043667287597</v>
+        <v>58.136791666666703</v>
       </c>
       <c r="I4">
-        <v>43.1766535663998</v>
+        <v>2.4264211253232499</v>
       </c>
       <c r="J4">
-        <v>0.47429845344238097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>410.61864000000003</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>840.86069999999995</v>
-      </c>
-      <c r="D6">
-        <v>5530.3360000000002</v>
-      </c>
-      <c r="E6">
-        <v>3.67414206545583E-2</v>
-      </c>
-      <c r="F6">
-        <v>1.26148301458118</v>
-      </c>
-      <c r="G6">
-        <v>68.241833333333304</v>
-      </c>
-      <c r="H6">
-        <v>4.8315806956443499</v>
-      </c>
-      <c r="I6">
-        <v>4.9458937661225804</v>
-      </c>
-      <c r="J6">
-        <v>0.100881407272675</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>654.34670000000006</v>
-      </c>
-      <c r="D7">
-        <v>4360.4979999999996</v>
-      </c>
-      <c r="E7">
-        <v>0.33558506980650299</v>
-      </c>
-      <c r="F7">
-        <v>197.52387140350299</v>
-      </c>
-      <c r="G7">
-        <v>58.136791666666703</v>
-      </c>
-      <c r="H7">
-        <v>0.95616784071764405</v>
-      </c>
-      <c r="I7">
-        <v>1.1733888577156899</v>
-      </c>
-      <c r="J7">
-        <v>2.2956195890375901</v>
+        <v>2.9776524490128899</v>
+      </c>
+      <c r="K4">
+        <v>0.47387400561080101</v>
       </c>
     </row>
   </sheetData>
@@ -8923,16 +8971,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8963,197 +9014,215 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>655.34429999999998</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1.5364385574572501</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.476041666698</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
+        <v>638.45846666666705</v>
+      </c>
+      <c r="E2">
         <v>3992.6460000000002</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.215852248068133</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>34.390505339251298</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>53.767708333333303</v>
       </c>
-      <c r="H2">
-        <v>0.42592403459915501</v>
-      </c>
       <c r="I2">
-        <v>0.56756507410637702</v>
+        <v>5.2289212652668198</v>
       </c>
       <c r="J2">
-        <v>1.5364385574572501</v>
+        <v>6.9677990541449004</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45484</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>779.41542000000004</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>1.6768239255734401</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45484.508796296301</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3">
+        <v>792.39509999999996</v>
+      </c>
+      <c r="E3">
         <v>8306.5229999999992</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.23609790544256401</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>47.514255157747101</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>76.441249999999997</v>
       </c>
-      <c r="H3">
-        <v>15.6852075034425</v>
-      </c>
       <c r="I3">
-        <v>13.9945930170877</v>
+        <v>37.9449411668583</v>
       </c>
       <c r="J3">
-        <v>1.6768239255734401</v>
+        <v>33.855083432652698</v>
+      </c>
+      <c r="K3">
+        <v>1.52962388841246</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>532.55862000000002</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>1.1028312072387401</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45590.410069444399</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>1052.144</v>
+        <v>546.66366000000005</v>
       </c>
       <c r="E4">
+        <v>1413.367</v>
+      </c>
+      <c r="F4">
         <v>0.16324969531057901</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>12.671592764002201</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>69.349500000000006</v>
       </c>
-      <c r="H4">
-        <v>19.818470739973201</v>
-      </c>
       <c r="I4">
-        <v>19.9019208028636</v>
+        <v>133.14792377377401</v>
       </c>
       <c r="J4">
-        <v>1.1028312072387401</v>
+        <v>133.70857261285099</v>
+      </c>
+      <c r="K4">
+        <v>2.1261592525806399</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>699.4171</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2.9322257640588401</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45279.458796296298</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
+        <v>743.79520000000002</v>
+      </c>
+      <c r="E5">
         <v>3992.6460000000002</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.52826006985347296</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>855.51132713685695</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>57.950125</v>
       </c>
-      <c r="H5">
-        <v>10.0849792289545</v>
-      </c>
       <c r="I5">
-        <v>12.417608085285099</v>
+        <v>24.594500550219902</v>
       </c>
       <c r="J5">
-        <v>2.9322257640588401</v>
+        <v>30.283143073723501</v>
+      </c>
+      <c r="K5">
+        <v>1.48120094839522</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>2.1111055589692098</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45502.467245370397</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <v>801.76949999999999</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4010.9160000000002</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.31201786247728303</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>129.15331535889499</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>76.383166666666696</v>
       </c>
-      <c r="H6">
-        <v>14.2836545918616</v>
-      </c>
       <c r="I6">
-        <v>12.7553315960599</v>
+        <v>106.92166975523401</v>
       </c>
       <c r="J6">
-        <v>2.1111055589692098</v>
+        <v>95.481261028916606</v>
+      </c>
+      <c r="K6">
+        <v>1.97991814613576</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>547.61717999999996</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>1.7653911789886501</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45569.420833333301</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
       <c r="D7">
+        <v>693.87467000000004</v>
+      </c>
+      <c r="E7">
         <v>6443.8360000000002</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.24996315545078601</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>58.262776767551102</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>76.3036666666667</v>
       </c>
-      <c r="H7">
-        <v>36.912859552156597</v>
-      </c>
       <c r="I7">
-        <v>33.0116836786571</v>
+        <v>262.11659900540798</v>
       </c>
       <c r="J7">
-        <v>1.7653911789886501</v>
+        <v>234.41451998769301</v>
+      </c>
+      <c r="K7">
+        <v>2.3699845090321801</v>
       </c>
     </row>
   </sheetData>
@@ -9164,16 +9233,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9204,194 +9273,177 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>473.84879999999998</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1.5901312641124601</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.610069444403</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
       <c r="D2">
+        <v>456.12386666666703</v>
+      </c>
+      <c r="E2">
         <v>6443.8360000000002</v>
       </c>
-      <c r="E2">
-        <v>0.41422688193861201</v>
-      </c>
       <c r="F2">
-        <v>39.2335750636623</v>
+        <v>0.41311509484043002</v>
       </c>
       <c r="G2">
-        <v>54.145791666666703</v>
+        <v>38.916275041201203</v>
       </c>
       <c r="H2">
-        <v>5.5558661720727098E-2</v>
+        <v>54.664183908045999</v>
       </c>
       <c r="I2">
-        <v>7.3504151522309297E-2</v>
+        <v>7.0654292394224605E-2</v>
       </c>
       <c r="J2">
-        <v>1.5936578839561699</v>
+        <v>9.2553841251804506E-2</v>
+      </c>
+      <c r="K2">
+        <v>-1.0336055520613401</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>1.3870902571252</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45590.473611111098</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
         <v>411.06707999999998</v>
       </c>
-      <c r="D3">
-        <v>3344.355</v>
-      </c>
       <c r="E3">
+        <v>5182.0039999999999</v>
+      </c>
+      <c r="F3">
         <v>0.35358594626280099</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>24.383175083471102</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>68.4775833333333</v>
       </c>
-      <c r="H3">
-        <v>0.30827126972012397</v>
-      </c>
       <c r="I3">
-        <v>0.31419620586510399</v>
+        <v>2.0998859841322499</v>
       </c>
       <c r="J3">
-        <v>1.3870902571252</v>
+        <v>2.1402455362209598</v>
+      </c>
+      <c r="K3">
+        <v>0.33046359994212099</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>730.71659999999997</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>1.2690811021975701</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45231.505902777797</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
       <c r="D4">
+        <v>714.04719999999998</v>
+      </c>
+      <c r="E4">
         <v>6744.4539999999997</v>
       </c>
-      <c r="E4">
-        <v>0.32268700082854701</v>
-      </c>
       <c r="F4">
-        <v>18.5265754025319</v>
+        <v>0.32300434886584101</v>
       </c>
       <c r="G4">
-        <v>67.036416666666696</v>
+        <v>18.581514226441701</v>
       </c>
       <c r="H4">
-        <v>2.11332013024744E-2</v>
+        <v>67.133880000000005</v>
       </c>
       <c r="I4">
-        <v>2.2090623667874398E-2</v>
+        <v>7.2729609680837304E-2</v>
       </c>
       <c r="J4">
-        <v>1.2677951483401999</v>
+        <v>7.5881613953076701E-2</v>
+      </c>
+      <c r="K4">
+        <v>-1.1198634405211101</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>699.4171</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="B5" s="1">
+        <v>45279.458796296298</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
       <c r="D5">
+        <v>743.79520000000002</v>
+      </c>
+      <c r="E5">
         <v>8053.1170000000002</v>
       </c>
-      <c r="E5">
-        <v>0.86567996287507698</v>
-      </c>
       <c r="F5">
-        <v>360.82578389464197</v>
+        <v>0.86743688694584598</v>
       </c>
       <c r="G5">
-        <v>58.517166666666697</v>
+        <v>363.04466107748698</v>
       </c>
       <c r="H5">
-        <v>1.73058886604297</v>
+        <v>58.592009009008997</v>
       </c>
       <c r="I5">
-        <v>2.1088768075705602</v>
+        <v>4.5489596822252896</v>
       </c>
       <c r="J5">
-        <v>2.5572975638008</v>
+        <v>5.5359116546346296</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45505</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>752.10996</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>1.4983746072415201</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45569.462962963</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>9327.6489999999994</v>
+        <v>395.82371999999998</v>
       </c>
       <c r="E6">
-        <v>0.39723668915869298</v>
+        <v>3225.154</v>
       </c>
       <c r="F6">
-        <v>34.6942253975892</v>
+        <v>0.38499526710283399</v>
       </c>
       <c r="G6">
-        <v>76.912333333333294</v>
+        <v>31.504646231116201</v>
       </c>
       <c r="H6">
-        <v>0.33865857049369802</v>
+        <v>75.438470588235305</v>
       </c>
       <c r="I6">
-        <v>0.29986232108031602</v>
+        <v>14.7789864366346</v>
       </c>
       <c r="J6">
-        <v>1.5402571956364199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>395.73576000000003</v>
-      </c>
-      <c r="D7">
-        <v>3225.154</v>
-      </c>
-      <c r="E7">
-        <v>0.38487369823224499</v>
-      </c>
-      <c r="F7">
-        <v>31.475139594695701</v>
-      </c>
-      <c r="G7">
-        <v>75.441000000000003</v>
-      </c>
-      <c r="H7">
-        <v>6.3222902982053197</v>
-      </c>
-      <c r="J7">
-        <v>1.4979676649140301</v>
+        <v>13.405106779878199</v>
+      </c>
+      <c r="K6">
+        <v>1.12727027775397</v>
       </c>
     </row>
   </sheetData>
@@ -9402,16 +9454,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9442,292 +9494,215 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45442</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>688.71222</v>
-      </c>
-      <c r="H2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I2" t="e">
-        <v>#NUM!</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>2.2638461049630898</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45484.417592592603</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>2034.8627879999999</v>
+      </c>
+      <c r="E2">
+        <v>6961.3969999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.25670942796431001</v>
+      </c>
+      <c r="G2">
+        <v>183.58876694917501</v>
+      </c>
+      <c r="H2">
+        <v>76.579041666666697</v>
+      </c>
+      <c r="I2">
+        <v>5.2363099452820601</v>
+      </c>
+      <c r="J2">
+        <v>4.6609674789689297</v>
+      </c>
+      <c r="K2">
+        <v>0.668476072734428</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45484</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>690.81389999999999</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2.21129687400897</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45296.400694444397</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>6961.3969999999999</v>
+        <v>426.60744999999997</v>
       </c>
       <c r="E3">
-        <v>0.25670942796431001</v>
+        <v>3375.2420000000002</v>
       </c>
       <c r="F3">
-        <v>183.58876694917501</v>
+        <v>0.225012367816944</v>
       </c>
       <c r="G3">
-        <v>76.579041666666697</v>
+        <v>162.66603244559099</v>
       </c>
       <c r="H3">
-        <v>4.7455135401012898</v>
+        <v>54.871041666666699</v>
       </c>
       <c r="I3">
-        <v>4.2240976016608602</v>
+        <v>4.6033147560070597</v>
       </c>
       <c r="J3">
-        <v>2.2638461049630898</v>
+        <v>6.0054934004881702</v>
+      </c>
+      <c r="K3">
+        <v>0.77854869405477301</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>548.14409999999998</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>2.0237147747062201</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45266.452662037002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>8635.2430000000004</v>
+        <v>409.7124</v>
       </c>
       <c r="E4">
-        <v>1.4553017535786799E-3</v>
+        <v>4325.9719999999998</v>
       </c>
       <c r="F4">
-        <v>1.5389269136462</v>
+        <v>0.14071662604863699</v>
       </c>
       <c r="G4">
-        <v>69.716999999999999</v>
+        <v>105.61236663593399</v>
       </c>
       <c r="H4">
-        <v>47.996062389961097</v>
+        <v>62.968666666666699</v>
+      </c>
+      <c r="I4">
+        <v>5.7587643197985896</v>
       </c>
       <c r="J4">
-        <v>0.18721799491019001</v>
+        <v>6.4695823800006398</v>
+      </c>
+      <c r="K4">
+        <v>0.81087624729699004</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>563.09195999999997</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#NUM!</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2.6628273408915302</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45279.417939814797</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>444.28</v>
+      </c>
+      <c r="E5">
+        <v>3363.2</v>
+      </c>
+      <c r="F5">
+        <v>0.69658739105357004</v>
+      </c>
+      <c r="G5">
+        <v>460.07362929256902</v>
+      </c>
+      <c r="H5">
+        <v>59.392708333333303</v>
+      </c>
+      <c r="I5">
+        <v>1.9236150869142301</v>
+      </c>
+      <c r="J5">
+        <v>2.3061402301815401</v>
+      </c>
+      <c r="K5">
+        <v>0.36288571204037201</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>429.05880000000002</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>2.45769239868789</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45502.410763888904</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>3375.2420000000002</v>
+        <v>1722.98714</v>
       </c>
       <c r="E6">
-        <v>0.225012367816944</v>
+        <v>6713.1440000000002</v>
       </c>
       <c r="F6">
-        <v>162.66603244559099</v>
+        <v>0.41694777291652502</v>
       </c>
       <c r="G6">
-        <v>54.871041666666699</v>
+        <v>286.87479906384101</v>
       </c>
       <c r="H6">
-        <v>0.425674054587034</v>
+        <v>76.361791666666704</v>
       </c>
       <c r="I6">
-        <v>0.55533520106256995</v>
+        <v>1.5113924672972501</v>
       </c>
       <c r="J6">
-        <v>2.21129687400897</v>
+        <v>1.3500727112072699</v>
+      </c>
+      <c r="K6">
+        <v>0.130357159032578</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45266</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>409.7124</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>1.7445663101922899</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45569.336458333302</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>4325.9719999999998</v>
+        <v>520.15418799999998</v>
       </c>
       <c r="E7">
-        <v>0.14071662604863699</v>
+        <v>8379.9380000000001</v>
       </c>
       <c r="F7">
-        <v>105.61236663593399</v>
+        <v>7.0018058078074194E-2</v>
       </c>
       <c r="G7">
-        <v>62.968666666666699</v>
+        <v>55.534940409272103</v>
       </c>
       <c r="H7">
-        <v>1.9954189154176001</v>
+        <v>75.600666666666697</v>
       </c>
       <c r="I7">
-        <v>2.2417182470070598</v>
+        <v>1.9735868782610999</v>
       </c>
       <c r="J7">
-        <v>2.0237147747062201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A8" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>444.28</v>
-      </c>
-      <c r="D8">
-        <v>3363.2</v>
-      </c>
-      <c r="E8">
-        <v>0.69658739105357004</v>
-      </c>
-      <c r="F8">
-        <v>460.07362929256902</v>
-      </c>
-      <c r="G8">
-        <v>59.392708333333303</v>
-      </c>
-      <c r="H8">
-        <v>0.79918461724656098</v>
-      </c>
-      <c r="I8">
-        <v>0.95810841249484902</v>
-      </c>
-      <c r="J8">
-        <v>2.6628273408915302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A9" s="1">
-        <v>45376</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>545.70809999999994</v>
-      </c>
-      <c r="D9">
-        <v>4021.9380000000001</v>
-      </c>
-      <c r="E9">
-        <v>0.140700754388522</v>
-      </c>
-      <c r="F9">
-        <v>105.53100859400401</v>
-      </c>
-      <c r="G9">
-        <v>62.832791666666701</v>
-      </c>
-      <c r="H9">
-        <v>0.58933237308338704</v>
-      </c>
-      <c r="I9">
-        <v>0.66357904524141798</v>
-      </c>
-      <c r="J9">
-        <v>2.0233800888523201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A10" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>776.96429999999998</v>
-      </c>
-      <c r="D10">
-        <v>6713.1440000000002</v>
-      </c>
-      <c r="E10">
-        <v>0.41694777291652502</v>
-      </c>
-      <c r="F10">
-        <v>286.87479906384101</v>
-      </c>
-      <c r="G10">
-        <v>76.361791666666704</v>
-      </c>
-      <c r="H10">
-        <v>0.65114613390860798</v>
-      </c>
-      <c r="I10">
-        <v>0.58164549937857801</v>
-      </c>
-      <c r="J10">
-        <v>2.45769239868789</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A11" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>395.84652</v>
-      </c>
-      <c r="D11">
-        <v>8379.9380000000001</v>
-      </c>
-      <c r="E11">
-        <v>7.0018058078074194E-2</v>
-      </c>
-      <c r="F11">
-        <v>55.534940409272103</v>
-      </c>
-      <c r="G11">
-        <v>75.600666666666697</v>
-      </c>
-      <c r="H11">
-        <v>0.33165288386252301</v>
-      </c>
-      <c r="I11">
-        <v>0.30002456976414499</v>
-      </c>
-      <c r="J11">
-        <v>1.7445663101922899</v>
+        <v>1.78537435630409</v>
       </c>
     </row>
   </sheetData>
@@ -9738,16 +9713,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9778,133 +9753,145 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>650.67600000000004</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1.1162597991251899</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.434953703698</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
       <c r="D2">
+        <v>618.29094999999995</v>
+      </c>
+      <c r="E2">
         <v>4929.4979999999996</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.42599051773861102</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>13.0695248584331</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>55.262291666666698</v>
       </c>
-      <c r="H2">
-        <v>0.59619442027784597</v>
-      </c>
       <c r="I2">
-        <v>0.772252348942841</v>
+        <v>1.45678128745316</v>
       </c>
       <c r="J2">
-        <v>1.1162597991251899</v>
+        <v>1.8869729954993399</v>
+      </c>
+      <c r="K2">
+        <v>0.275765685014141</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>835.77359999999999</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>0.83364298367996603</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45590.382638888899</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>7282.4489999999996</v>
+        <v>921.71709999999996</v>
       </c>
       <c r="E3">
+        <v>4210.08</v>
+      </c>
+      <c r="F3">
         <v>0.35046535211951502</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6.8177800097671497</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>68.263083333333299</v>
       </c>
-      <c r="H3">
-        <v>2.1767630223752299</v>
-      </c>
       <c r="I3">
-        <v>2.22687990873807</v>
+        <v>42.888077344183998</v>
       </c>
       <c r="J3">
-        <v>0.83364298367996603</v>
+        <v>43.875514596877601</v>
+      </c>
+      <c r="K3">
+        <v>1.6422222231553301</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>402.31270000000001</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>0.88643327723876397</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45231.413888888899</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
+        <v>434.69794999999999</v>
+      </c>
+      <c r="E4">
         <v>17383.669999999998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.36326953896331998</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7.6989815209433896</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>67.299833333333297</v>
       </c>
-      <c r="H4">
-        <v>0.32657792786206402</v>
-      </c>
       <c r="I4">
-        <v>0.33977184565730401</v>
+        <v>0.80706235080412003</v>
       </c>
       <c r="J4">
-        <v>0.88643327723876397</v>
+        <v>0.83966808868068499</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>547.30542000000003</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>0.97707971959916795</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45569.400115740696</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
       <c r="D5">
+        <v>555.11051999999995</v>
+      </c>
+      <c r="E5">
         <v>14306.2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.386909393539067</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>9.4859257207413101</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>75.319166666666703</v>
       </c>
-      <c r="H5">
-        <v>1.0342626178979999</v>
-      </c>
       <c r="I5">
-        <v>0.93977831967298397</v>
+        <v>7.8376760318942296</v>
       </c>
       <c r="J5">
-        <v>0.97707971959916795</v>
+        <v>7.12167092180563</v>
+      </c>
+      <c r="K5">
+        <v>0.85258190192095995</v>
       </c>
     </row>
   </sheetData>
@@ -9915,16 +9902,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9955,289 +9942,285 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>644.81269999999995</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>2.20683808773562</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.650231481501</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
       <c r="D2">
+        <v>612.31027500000005</v>
+      </c>
+      <c r="E2">
         <v>7115.5159999999996</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.28772677954446901</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>161.004527140063</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>57.347416666666703</v>
       </c>
-      <c r="H2">
-        <v>0.93227266845144696</v>
-      </c>
       <c r="I2">
-        <v>1.1610877322831099</v>
+        <v>2.2976376979999702</v>
       </c>
       <c r="J2">
-        <v>2.20683808773562</v>
+        <v>2.8615651135737599</v>
+      </c>
+      <c r="K2">
+        <v>0.45660363252434699</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45442</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>645.07506000000001</v>
-      </c>
-      <c r="H3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#NUM!</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2.0309945857151401</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45590.509490740696</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>509.79309000000001</v>
+      </c>
+      <c r="E3">
+        <v>9416.6620000000003</v>
+      </c>
+      <c r="F3">
+        <v>0.21002135752523299</v>
+      </c>
+      <c r="G3">
+        <v>107.397602315806</v>
+      </c>
+      <c r="H3">
+        <v>68.863500000000002</v>
+      </c>
+      <c r="I3">
+        <v>28.964352921548802</v>
+      </c>
+      <c r="J3">
+        <v>29.329684647404299</v>
+      </c>
+      <c r="K3">
+        <v>1.46730739347396</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45484</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>20605.830000000002</v>
-      </c>
-      <c r="H4" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I4" t="e">
-        <v>#NUM!</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>1.8044538113953601</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45597.442013888904</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>709.25940000000003</v>
+      </c>
+      <c r="E4">
+        <v>9416.6620000000003</v>
+      </c>
+      <c r="F4">
+        <v>0.14001852958251401</v>
+      </c>
+      <c r="G4">
+        <v>63.7461281387246</v>
+      </c>
+      <c r="H4">
+        <v>69.199291666666696</v>
+      </c>
+      <c r="I4">
+        <v>13183.643157193201</v>
+      </c>
+      <c r="J4">
+        <v>13271.8369261322</v>
+      </c>
+      <c r="K4">
+        <v>4.12293103678092</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>502.29234000000002</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>1.1421668183018401</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45618.515393518501</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>11548.536</v>
+        <v>2030.428296</v>
       </c>
       <c r="E5">
-        <v>0.21002135752523299</v>
+        <v>9416.6620000000003</v>
       </c>
       <c r="F5">
-        <v>107.397602315806</v>
+        <v>4.2821005642011099E-2</v>
       </c>
       <c r="G5">
-        <v>68.863500000000002</v>
+        <v>13.8728860259441</v>
       </c>
       <c r="H5">
-        <v>2.9986991093865498</v>
+        <v>65.772230769230802</v>
       </c>
       <c r="I5">
-        <v>3.0365221508306601</v>
+        <v>345.58511102516297</v>
       </c>
       <c r="J5">
-        <v>2.0309945857151401</v>
+        <v>369.30611714530801</v>
+      </c>
+      <c r="K5">
+        <v>2.5673865013158799</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>608.31299999999999</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>1.4499582859448901</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45266.611111111102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
       <c r="D6">
+        <v>615.23294999999996</v>
+      </c>
+      <c r="E6">
+        <v>10319.43</v>
+      </c>
+      <c r="F6">
+        <v>7.4268725880109507E-2</v>
+      </c>
+      <c r="G6">
+        <v>28.181122381291299</v>
+      </c>
+      <c r="H6">
+        <v>63.182749999999999</v>
+      </c>
+      <c r="I6">
+        <v>2.9840551192787101</v>
+      </c>
+      <c r="J6">
+        <v>3.3393862336951301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>1.96604947122087</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45331.457060185203</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>504.21780863999999</v>
+      </c>
+      <c r="E7">
+        <v>12721.81</v>
+      </c>
+      <c r="F7">
+        <v>0.18695286733230901</v>
+      </c>
+      <c r="G7">
+        <v>92.480351387484305</v>
+      </c>
+      <c r="H7">
+        <v>56.771625</v>
+      </c>
+      <c r="I7">
+        <v>10.1233281358362</v>
+      </c>
+      <c r="J7">
+        <v>12.744682901726801</v>
+      </c>
+      <c r="K7">
+        <v>1.10532903433306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>1.8159109638656199</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45502.5288194444</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2747.5827119999999</v>
+      </c>
+      <c r="E8">
         <v>9416.6620000000003</v>
       </c>
-      <c r="E6">
-        <v>0.14001852958251401</v>
-      </c>
-      <c r="F6">
-        <v>63.7461281387246</v>
-      </c>
-      <c r="G6">
-        <v>69.199291666666696</v>
-      </c>
-      <c r="H6">
-        <v>2256.79613620903</v>
-      </c>
-      <c r="J6">
-        <v>1.8044538113953601</v>
+      <c r="F8">
+        <v>0.117907274695669</v>
+      </c>
+      <c r="G8">
+        <v>65.450197871718402</v>
+      </c>
+      <c r="H8">
+        <v>74.329666666666697</v>
+      </c>
+      <c r="I8">
+        <v>47.814199417273002</v>
+      </c>
+      <c r="J8">
+        <v>44.159388507899898</v>
+      </c>
+      <c r="K8">
+        <v>1.6450230509194299</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>698.6585</v>
-      </c>
-      <c r="D7">
-        <v>11130.56</v>
-      </c>
-      <c r="E7">
-        <v>8.2976287770757301E-2</v>
-      </c>
-      <c r="F7">
-        <v>32.522982093317097</v>
-      </c>
-      <c r="G7">
-        <v>68.278565217391304</v>
-      </c>
-      <c r="H7">
-        <v>0.33341510601558799</v>
-      </c>
-      <c r="I7">
-        <v>0.34109151672638899</v>
-      </c>
-      <c r="J7">
-        <v>1.5121903600245801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A8" s="1">
-        <v>45266</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>595.43700000000001</v>
-      </c>
-      <c r="D8">
-        <v>10319.43</v>
-      </c>
-      <c r="E8">
-        <v>7.4268725880109507E-2</v>
-      </c>
-      <c r="F8">
-        <v>28.181122381291299</v>
-      </c>
-      <c r="G8">
-        <v>63.182749999999999</v>
-      </c>
-      <c r="H8">
-        <v>0.38300537388112299</v>
-      </c>
-      <c r="I8">
-        <v>0.42861234858122599</v>
-      </c>
-      <c r="J8">
-        <v>1.4499582859448901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A9" s="1">
-        <v>45331</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>433.461546</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>2.1665711356348201</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45569.486458333296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>10290.9</v>
+        <v>1103.890144</v>
       </c>
       <c r="E9">
-        <v>0.18695286733230901</v>
+        <v>9416.6620000000003</v>
       </c>
       <c r="F9">
-        <v>92.480351387484305</v>
+        <v>0.26756115791951901</v>
       </c>
       <c r="G9">
-        <v>56.771625</v>
+        <v>146.747643377652</v>
       </c>
       <c r="H9">
-        <v>5.1700820436274597</v>
+        <v>75.326458333333306</v>
       </c>
       <c r="I9">
-        <v>6.5088333933078397</v>
+        <v>3.6052078189927501</v>
       </c>
       <c r="J9">
-        <v>1.96604947122087</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A10" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
-        <v>667.35563999999999</v>
-      </c>
-      <c r="D10">
-        <v>9438.768</v>
-      </c>
-      <c r="E10">
-        <v>0.142858205716412</v>
-      </c>
-      <c r="F10">
-        <v>65.450197871718402</v>
-      </c>
-      <c r="G10">
-        <v>74.173434782608695</v>
-      </c>
-      <c r="H10">
-        <v>23.488344169076299</v>
-      </c>
-      <c r="J10">
-        <v>1.8159109638656199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A11" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>395.63819999999998</v>
-      </c>
-      <c r="D11">
-        <v>10445.418</v>
-      </c>
-      <c r="E11">
-        <v>0.26756115791951901</v>
-      </c>
-      <c r="F11">
-        <v>146.747643377652</v>
-      </c>
-      <c r="G11">
-        <v>75.326458333333306</v>
-      </c>
-      <c r="H11">
-        <v>1.0288636078548099</v>
-      </c>
-      <c r="I11">
-        <v>0.93487253220809396</v>
-      </c>
-      <c r="J11">
-        <v>2.1665711356348201</v>
+        <v>3.27585671914813</v>
+      </c>
+      <c r="K9">
+        <v>0.51532489814205995</v>
       </c>
     </row>
   </sheetData>
@@ -10248,16 +10231,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" activeCellId="1" sqref="A1:A1048576 K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10288,127 +10271,148 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>411.13853999999998</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>-0.70444482698631605</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45590.492476851898</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>19886.63</v>
+        <v>505.04641199999998</v>
       </c>
       <c r="E2">
+        <v>12559.68</v>
+      </c>
+      <c r="F2">
         <v>3.0144859170837299E-2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.19749457616861299</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>67.998583333333301</v>
       </c>
-      <c r="H2">
-        <v>16.1343103460324</v>
-      </c>
       <c r="I2">
-        <v>16.5829663340247</v>
+        <v>204.408460187423</v>
+      </c>
+      <c r="J2">
+        <v>210.092563052218</v>
+      </c>
+      <c r="K2">
+        <v>2.3224106793333701</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>-0.427984615686272</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45296.649884259299</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
         <v>637.03409999999997</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>9416.6620000000003</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3.9374423084510397E-2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.37326337992833297</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>52.158749999999998</v>
       </c>
-      <c r="H3">
-        <v>4.36213642925469</v>
-      </c>
       <c r="I3">
-        <v>5.99346173557774</v>
+        <v>9.6792073185934395</v>
+      </c>
+      <c r="J3">
+        <v>13.298978524756</v>
+      </c>
+      <c r="K3">
+        <v>1.1238182847190901</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>647.25275999999997</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>0.489735658561678</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45502.510416666701</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
       <c r="D4">
+        <v>718.57919000000004</v>
+      </c>
+      <c r="E4">
         <v>20938.13</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>9.2340088456400696E-2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3.0884150388744702</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>76.433750000000003</v>
       </c>
-      <c r="H4">
-        <v>0.47263363728687002</v>
-      </c>
       <c r="I4">
-        <v>0.42169129089072499</v>
+        <v>3.53500894211804</v>
       </c>
       <c r="J4">
-        <v>0.489735658561678</v>
+        <v>3.1539915200898601</v>
+      </c>
+      <c r="K4">
+        <v>0.49886052133811898</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>801.09990000000005</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2.01966151161424</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45279.534722222197</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5">
+        <v>811.21124999999995</v>
+      </c>
+      <c r="E5">
         <v>7747.7939999999999</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.38613206590049598</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>104.63127357915801</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>57.410541666666703</v>
       </c>
-      <c r="H5">
-        <v>2.1870162654264998E-2</v>
-      </c>
       <c r="I5">
-        <v>2.7201304818480699E-2</v>
+        <v>9.3657584724838594E-2</v>
       </c>
       <c r="J5">
-        <v>2.01966151161424</v>
+        <v>0.116487862981952</v>
+      </c>
+      <c r="K5">
+        <v>-0.93371932197318797</v>
       </c>
     </row>
   </sheetData>
@@ -10419,16 +10423,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10459,197 +10463,180 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>679.72839999999997</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1.4174733368758401</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.551157407397</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
       </c>
       <c r="D2">
+        <v>669.22050000000002</v>
+      </c>
+      <c r="E2">
         <v>8812.9509999999991</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.242294433819637</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>26.1500989699855</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>57.088374999999999</v>
       </c>
-      <c r="H2">
-        <v>0.24390358452308999</v>
-      </c>
       <c r="I2">
-        <v>0.30520205545490398</v>
+        <v>1.7502448346720501</v>
       </c>
       <c r="J2">
-        <v>1.4174733368758401</v>
+        <v>2.19012083047377</v>
+      </c>
+      <c r="K2">
+        <v>0.34046807582660699</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>441.74369999999999</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>1.27952656840493</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45590.450462963003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>2526.8760000000002</v>
+        <v>441.72498000000002</v>
       </c>
       <c r="E3">
-        <v>0.218316630467253</v>
+        <v>2233.951</v>
       </c>
       <c r="F3">
+        <v>0.16002503851161501</v>
+      </c>
+      <c r="G3">
         <v>19.033846755006099</v>
       </c>
-      <c r="G3">
-        <v>69.479695652173902</v>
-      </c>
       <c r="H3">
-        <v>1.9939050567780701</v>
+        <v>69.406999999999996</v>
       </c>
       <c r="I3">
-        <v>1.99799058223319</v>
+        <v>7.6800051194760899</v>
       </c>
       <c r="J3">
-        <v>1.27952656840493</v>
+        <v>7.7052219258119203</v>
+      </c>
+      <c r="K3">
+        <v>0.88678515178480999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>719.91600000000005</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>0.60666256556119902</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45231.5222222222</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
       </c>
       <c r="D4">
+        <v>744.31614999999999</v>
+      </c>
+      <c r="E4">
         <v>4485.2950000000001</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.13055244711888001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4.0426166984303</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>68.842375000000004</v>
       </c>
-      <c r="H4">
-        <v>0.46872140092199499</v>
-      </c>
       <c r="I4">
-        <v>0.47478024802958502</v>
+        <v>3.6775252589669298</v>
       </c>
       <c r="J4">
-        <v>0.60666256556119902</v>
+        <v>3.7250621609188102</v>
+      </c>
+      <c r="K4">
+        <v>0.57113352431083098</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45279</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>418.92230000000001</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>2.8626748394097299</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45279.418749999997</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
       <c r="D5">
+        <v>452.6567</v>
+      </c>
+      <c r="E5">
         <v>9377.6460000000006</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.73138680186451299</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>728.91156257831699</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>60.173708333333302</v>
       </c>
-      <c r="H5">
-        <v>0.23444114467744401</v>
-      </c>
       <c r="I5">
-        <v>0.27708508441848401</v>
+        <v>0.58631953021781402</v>
       </c>
       <c r="J5">
-        <v>2.8626748394097299</v>
+        <v>0.69296879073905904</v>
+      </c>
+      <c r="K5">
+        <v>-0.15928632428432901</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45505</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>642.23753999999997</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>1.52582427682962</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45569.448379629597</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>3474.2550000000001</v>
+        <v>373.09719000000001</v>
       </c>
       <c r="E6">
-        <v>0.26661213979770598</v>
+        <v>1201.4880000000001</v>
       </c>
       <c r="F6">
-        <v>35.070620539330598</v>
+        <v>0.26345251809384701</v>
       </c>
       <c r="G6">
-        <v>76.782291666666694</v>
+        <v>33.5601796390159</v>
       </c>
       <c r="H6">
-        <v>4.0239547132744997</v>
+        <v>76.006291666666698</v>
       </c>
       <c r="I6">
-        <v>3.5702893922979699</v>
+        <v>18.702897913160601</v>
       </c>
       <c r="J6">
-        <v>1.54494345035321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>365.72465999999997</v>
-      </c>
-      <c r="D7">
-        <v>1201.4880000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.26345251809384701</v>
-      </c>
-      <c r="F7">
-        <v>33.5601796390159</v>
-      </c>
-      <c r="G7">
-        <v>76.006291666666698</v>
-      </c>
-      <c r="H7">
-        <v>2.6424089665535599</v>
-      </c>
-      <c r="I7">
-        <v>2.3742812408469902</v>
-      </c>
-      <c r="J7">
-        <v>1.52582427682962</v>
+        <v>16.805097252834202</v>
       </c>
     </row>
   </sheetData>
@@ -10660,16 +10647,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10700,240 +10687,264 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A2" s="1">
-        <v>45296</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>699.58140000000003</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>2.21964731557483</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45296.691319444399</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
       </c>
       <c r="D2">
+        <v>680.57703333333302</v>
+      </c>
+      <c r="E2">
         <v>4167.0529999999999</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.304619300450722</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>165.823972739732</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>52.267458333333302</v>
       </c>
-      <c r="H2">
-        <v>1.3297639505519001</v>
-      </c>
       <c r="I2">
-        <v>1.82328254299512</v>
+        <v>3.2423941808893599</v>
       </c>
       <c r="J2">
-        <v>2.21964731557483</v>
+        <v>4.4457519735520696</v>
+      </c>
+      <c r="K2">
+        <v>0.64794522995038195</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A3" s="1">
-        <v>45590</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>380.19384000000002</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>1.93082107397803</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45590.536805555603</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>385.73862000000003</v>
       </c>
       <c r="E3">
+        <v>11406.38</v>
+      </c>
+      <c r="F3">
         <v>0.189070453385662</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>85.274871565359604</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>67.770875000000004</v>
       </c>
+      <c r="I3">
+        <v>2.2494895291891299</v>
+      </c>
       <c r="J3">
-        <v>1.93082107397803</v>
+        <v>2.3214288357792698</v>
+      </c>
+      <c r="K3">
+        <v>0.36575537475554798</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A4" s="1">
-        <v>45597</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>365.95895999999999</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>1.7498332898101401</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45597.512847222199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>366.03865999999999</v>
       </c>
       <c r="E4">
+        <v>3957.6080000000002</v>
+      </c>
+      <c r="F4">
         <v>0.14022503226824601</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>56.212550380179103</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>68.742208333333295</v>
       </c>
+      <c r="I4">
+        <v>5.98707457535708</v>
+      </c>
       <c r="J4">
-        <v>1.7498332898101401</v>
+        <v>6.0757335254178502</v>
+      </c>
+      <c r="K4">
+        <v>0.78359871795927805</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A5" s="1">
-        <v>45231</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>721.23059999999998</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>1.41438658720066</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45618.559143518498</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>2687.3130000000001</v>
-      </c>
-      <c r="E5">
-        <v>0.1019830414486</v>
+        <v>2122.394256</v>
       </c>
       <c r="F5">
-        <v>36.054074208547597</v>
+        <v>8.0595708464144294E-2</v>
       </c>
       <c r="G5">
-        <v>65.837708333333296</v>
+        <v>25.9648959876038</v>
       </c>
       <c r="H5">
-        <v>1.82495889091172</v>
-      </c>
-      <c r="I5">
-        <v>1.9477536276551799</v>
-      </c>
-      <c r="J5">
-        <v>1.55695434828742</v>
+        <v>56.772214285714298</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A6" s="1">
-        <v>45266</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>739.46839999999997</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>1.5008062130991799</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45266.638425925899</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
       <c r="D6">
+        <v>711.255675</v>
+      </c>
+      <c r="E6">
         <v>3986.5630000000001</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>9.2948582820242806E-2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>31.6815348320814</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>57.605125000000001</v>
       </c>
-      <c r="H6">
-        <v>0.21060279927259001</v>
-      </c>
       <c r="I6">
-        <v>0.26097334154129898</v>
-      </c>
-      <c r="J6">
-        <v>1.5008062130991799</v>
+        <v>1.7493497646667899</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A7" s="1">
-        <v>45331</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>447.77111400000001</v>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>2.1287362422670499</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45331.513657407399</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
       <c r="D7">
+        <v>464.2354962</v>
+      </c>
+      <c r="E7">
         <v>3393.52</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.26214009253193299</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>134.504322807786</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>55.680374999999998</v>
       </c>
-      <c r="H7">
-        <v>36.698976971219601</v>
-      </c>
-      <c r="J7">
-        <v>2.1287362422670499</v>
+      <c r="I7">
+        <v>247.73184212307299</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A8" s="1">
-        <v>45502</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>719.93502000000001</v>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>1.78970531724707</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45502.6175925926</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
       </c>
       <c r="D8">
+        <v>703.29944999999998</v>
+      </c>
+      <c r="E8">
         <v>5518.3209999999999</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.14969712289074899</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>61.617676426121797</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>77.678708333333304</v>
       </c>
-      <c r="H8">
-        <v>2.54253644329191</v>
-      </c>
       <c r="I8">
-        <v>2.2231410310497299</v>
+        <v>18.435644843616998</v>
       </c>
       <c r="J8">
-        <v>1.78970531724707</v>
+        <v>16.119744750891499</v>
+      </c>
+      <c r="K8">
+        <v>1.2073581606603301</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
-      <c r="A9" s="1">
-        <v>45569</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>396.4812</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>1.94544135577539</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45569.557407407403</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>8222.7630000000008</v>
+        <v>403.84739999999999</v>
       </c>
       <c r="E9">
+        <v>8906.6890000000003</v>
+      </c>
+      <c r="F9">
         <v>0.19368252554686899</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>88.194470217674905</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>76.782666666666699</v>
       </c>
-      <c r="H9">
-        <v>0.488676963637731</v>
-      </c>
       <c r="I9">
-        <v>0.43358295603590602</v>
+        <v>3.5288640506226399</v>
       </c>
       <c r="J9">
-        <v>1.94544135577539</v>
+        <v>3.1310158251127902</v>
+      </c>
+      <c r="K9">
+        <v>0.49568526267976798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>